<commit_message>
Update 2025_2026 project self-evaluation spreadsheet
Revised the contents of the 2025_2026_proj_auto_avaliacao.xlsx file. Details of the changes are in the updated spreadsheet.
</commit_message>
<xml_diff>
--- a/RC_entrega/2025_2026_proj_auto_avaliacao.xlsx
+++ b/RC_entrega/2025_2026_proj_auto_avaliacao.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IST\2025-11-Redes-de-Computadores\AutoAvaliacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1FBD04-C4C0-495B-BC2C-CEF500807890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8A475D8-B625-47D4-A087-4A657C818E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="ewewq">lists!$G$24:$G$26</definedName>
     <definedName name="turnos" localSheetId="1">Table2[[#Headers],[turnos]]</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,6 +33,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +42,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
+  <si>
+    <t>Redes de Computadores 2025/2026</t>
+  </si>
   <si>
     <t>Ficha de autoavaliação</t>
   </si>
@@ -48,163 +53,45 @@
     <t>(ver descrição de cada teste no ficheiro PDF)</t>
   </si>
   <si>
-    <t>script 1</t>
-  </si>
-  <si>
-    <t>script 2</t>
-  </si>
-  <si>
-    <t>script 3</t>
-  </si>
-  <si>
-    <t>script 4</t>
-  </si>
-  <si>
-    <t>script 5</t>
-  </si>
-  <si>
-    <t>script 6</t>
-  </si>
-  <si>
-    <t>script 7</t>
-  </si>
-  <si>
-    <t>script 8</t>
-  </si>
-  <si>
-    <t>script 9</t>
-  </si>
-  <si>
-    <t>script 10</t>
-  </si>
-  <si>
-    <t>script 11</t>
+    <t>Identificação                          Turno</t>
   </si>
   <si>
     <t>Grupo</t>
   </si>
   <si>
-    <t>turnos</t>
-  </si>
-  <si>
     <t>Auto-aval</t>
   </si>
   <si>
-    <t>max 05</t>
-  </si>
-  <si>
-    <t>max 1</t>
-  </si>
-  <si>
-    <t>max 2</t>
-  </si>
-  <si>
-    <t>Observações:</t>
-  </si>
-  <si>
-    <t>script 21</t>
-  </si>
-  <si>
-    <t>script 22</t>
-  </si>
-  <si>
-    <t>script 23</t>
-  </si>
-  <si>
-    <t>script 24</t>
-  </si>
-  <si>
-    <t>script 25</t>
-  </si>
-  <si>
-    <t>script 26</t>
-  </si>
-  <si>
-    <t>Resposta</t>
-  </si>
-  <si>
-    <t>Completo</t>
-  </si>
-  <si>
-    <t>Quase completo</t>
-  </si>
-  <si>
-    <t>Incompleto</t>
-  </si>
-  <si>
-    <t>Não implementado</t>
-  </si>
-  <si>
-    <t>Identificação                          Turno</t>
-  </si>
-  <si>
-    <t>RC-3T02</t>
-  </si>
-  <si>
-    <t>RC-3T03</t>
-  </si>
-  <si>
-    <t>RC-3T04</t>
-  </si>
-  <si>
-    <t>RC-3T07</t>
-  </si>
-  <si>
-    <t>RC-3T08</t>
-  </si>
-  <si>
-    <t>RC-3T09</t>
-  </si>
-  <si>
-    <t>RC-3T10</t>
-  </si>
-  <si>
-    <t>RC-3T13</t>
-  </si>
-  <si>
-    <t>RC-3T14</t>
-  </si>
-  <si>
-    <t>RC-3T15</t>
-  </si>
-  <si>
-    <t>RC-3T16</t>
-  </si>
-  <si>
-    <t>RC-3T17</t>
-  </si>
-  <si>
-    <t>RC-3T18</t>
-  </si>
-  <si>
-    <t>Teste User – TCP (geral)</t>
-  </si>
-  <si>
-    <t>Teste User – UDP (Geral)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1- login UID password </t>
-  </si>
-  <si>
-    <t>13- Robustez (ciclo read/write; tamanho buffers, ...)</t>
-  </si>
-  <si>
-    <t>26- Robustez (ciclo read/write; múltiplos pedidos; ...)</t>
-  </si>
-  <si>
-    <t>script 12</t>
-  </si>
-  <si>
-    <t>script 27</t>
-  </si>
-  <si>
-    <t>script 28</t>
-  </si>
-  <si>
-    <t>script 29</t>
-  </si>
-  <si>
-    <t>Redes de Computadores 2025/2026</t>
+    <t>Cliente UDP (3,5 valores)</t>
+  </si>
+  <si>
+    <t>Servidor UDP (3,5 valores)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Interação </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – ES (UDP)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -233,33 +120,52 @@
     </r>
   </si>
   <si>
-    <t>Interação User – Servidor ES (TCP)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Interação </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>User</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> – ES (UDP)</t>
-    </r>
+    <t xml:space="preserve">1- login UID password </t>
+  </si>
+  <si>
+    <t>14- User faz login</t>
+  </si>
+  <si>
+    <t>2- myevents ou mye</t>
+  </si>
+  <si>
+    <t>15- User pede lista de eventos criados por si</t>
+  </si>
+  <si>
+    <t>3- myreservations ou myr</t>
+  </si>
+  <si>
+    <t>16- User pede lista de reservas que fez</t>
+  </si>
+  <si>
+    <t>4- logout</t>
+  </si>
+  <si>
+    <t>17- User faz logout</t>
+  </si>
+  <si>
+    <t>5- unregister</t>
+  </si>
+  <si>
+    <t>18- User faz unregister</t>
+  </si>
+  <si>
+    <t>Teste User – UDP (Geral)</t>
+  </si>
+  <si>
+    <t>Teste Servidor ES – UDP (Geral)</t>
+  </si>
+  <si>
+    <t>6- Robustez (select, timer, mens. incorretas)</t>
+  </si>
+  <si>
+    <t>19- Robustez (falhas comunicação; mens. incorretas)</t>
+  </si>
+  <si>
+    <t>Cliente TCP (7 valores)</t>
+  </si>
+  <si>
+    <t>Servidor TCP (6 valores)</t>
   </si>
   <si>
     <r>
@@ -288,94 +194,190 @@
     </r>
   </si>
   <si>
+    <t>Interação User – Servidor ES (TCP)</t>
+  </si>
+  <si>
+    <t>7- create event</t>
+  </si>
+  <si>
+    <t>20- User pede para iniciar um evento</t>
+  </si>
+  <si>
+    <t>8- close EID</t>
+  </si>
+  <si>
+    <t>21- User pede para fechar um evento</t>
+  </si>
+  <si>
+    <t>9- List</t>
+  </si>
+  <si>
+    <t>22- User pede a lists dos eventos</t>
+  </si>
+  <si>
+    <t>10- show EID</t>
+  </si>
+  <si>
+    <t>23- User pede ficheiro de descrição do evento (show)</t>
+  </si>
+  <si>
+    <t>11- RID EID</t>
+  </si>
+  <si>
+    <t>24- User faz reserva</t>
+  </si>
+  <si>
+    <t>12- Change Password</t>
+  </si>
+  <si>
+    <t>25- User faz "Change Password"</t>
+  </si>
+  <si>
+    <t>Teste User – TCP (geral)</t>
+  </si>
+  <si>
+    <t>Teste Servidor ES – TCP (Geral)</t>
+  </si>
+  <si>
+    <t>13- Robustez (ciclo read/write; tamanho buffers, ...)</t>
+  </si>
+  <si>
+    <t>26- Robustez (ciclo read/write; múltiplos pedidos; ...)</t>
+  </si>
+  <si>
+    <t>Observações:</t>
+  </si>
+  <si>
     <t>Execução correta dos scripts de testes do sevidor ES:</t>
   </si>
   <si>
-    <t>2- myevents ou mye</t>
-  </si>
-  <si>
-    <t>3- myreservations ou myr</t>
-  </si>
-  <si>
-    <t>4- logout</t>
-  </si>
-  <si>
-    <t>5- unregister</t>
-  </si>
-  <si>
-    <t>Cliente TCP (7 valores)</t>
-  </si>
-  <si>
-    <t>Servidor TCP (6 valores)</t>
-  </si>
-  <si>
-    <t>6- Robustez (select, timer, mens. incorretas)</t>
-  </si>
-  <si>
-    <t>7- create event</t>
-  </si>
-  <si>
-    <t>8- close EID</t>
-  </si>
-  <si>
-    <t>9- List</t>
-  </si>
-  <si>
-    <t>10- show EID</t>
-  </si>
-  <si>
-    <t>11- RID EID</t>
-  </si>
-  <si>
-    <t>12- Change Password</t>
-  </si>
-  <si>
-    <t>14- User faz login</t>
-  </si>
-  <si>
-    <t>15- User pede lista de eventos criados por si</t>
-  </si>
-  <si>
-    <t>17- User faz logout</t>
-  </si>
-  <si>
-    <t>18- User faz unregister</t>
-  </si>
-  <si>
-    <t>19- Robustez (falhas comunicação; mens. incorretas)</t>
-  </si>
-  <si>
-    <t>20- User pede para iniciar um evento</t>
-  </si>
-  <si>
-    <t>21- User pede para fechar um evento</t>
-  </si>
-  <si>
-    <t>22- User pede a lists dos eventos</t>
-  </si>
-  <si>
-    <t>23- User pede ficheiro de descrição do evento (show)</t>
-  </si>
-  <si>
-    <t>24- User faz reserva</t>
-  </si>
-  <si>
-    <t>25- User faz "Change Password"</t>
-  </si>
-  <si>
-    <t>Cliente UDP (3,5 valores)</t>
-  </si>
-  <si>
-    <t>Servidor UDP (3,5 valores)</t>
-  </si>
-  <si>
-    <t>16- User pede lista de reservas que fez</t>
-  </si>
-  <si>
-    <t>Teste Servidor ES – UDP (Geral)</t>
-  </si>
-  <si>
-    <t>Teste Servidor ES – TCP (Geral)</t>
+    <t>script 1</t>
+  </si>
+  <si>
+    <t>Completo</t>
+  </si>
+  <si>
+    <t>script 2</t>
+  </si>
+  <si>
+    <t>script 3</t>
+  </si>
+  <si>
+    <t>script 4</t>
+  </si>
+  <si>
+    <t>script 5</t>
+  </si>
+  <si>
+    <t>script 6</t>
+  </si>
+  <si>
+    <t>script 7</t>
+  </si>
+  <si>
+    <t>script 8</t>
+  </si>
+  <si>
+    <t>script 9</t>
+  </si>
+  <si>
+    <t>script 10</t>
+  </si>
+  <si>
+    <t>script 11</t>
+  </si>
+  <si>
+    <t>script 12</t>
+  </si>
+  <si>
+    <t>script 21</t>
+  </si>
+  <si>
+    <t>script 22</t>
+  </si>
+  <si>
+    <t>script 23</t>
+  </si>
+  <si>
+    <t>script 24</t>
+  </si>
+  <si>
+    <t>script 25</t>
+  </si>
+  <si>
+    <t>script 26</t>
+  </si>
+  <si>
+    <t>script 27</t>
+  </si>
+  <si>
+    <t>script 28</t>
+  </si>
+  <si>
+    <t>script 29</t>
+  </si>
+  <si>
+    <t>turnos</t>
+  </si>
+  <si>
+    <t>max 05</t>
+  </si>
+  <si>
+    <t>max 1</t>
+  </si>
+  <si>
+    <t>max 2</t>
+  </si>
+  <si>
+    <t>Resposta</t>
+  </si>
+  <si>
+    <t>RC-3T02</t>
+  </si>
+  <si>
+    <t>RC-3T03</t>
+  </si>
+  <si>
+    <t>Quase completo</t>
+  </si>
+  <si>
+    <t>RC-3T04</t>
+  </si>
+  <si>
+    <t>Incompleto</t>
+  </si>
+  <si>
+    <t>RC-3T07</t>
+  </si>
+  <si>
+    <t>Não implementado</t>
+  </si>
+  <si>
+    <t>RC-3T08</t>
+  </si>
+  <si>
+    <t>RC-3T09</t>
+  </si>
+  <si>
+    <t>RC-3T10</t>
+  </si>
+  <si>
+    <t>RC-3T13</t>
+  </si>
+  <si>
+    <t>RC-3T14</t>
+  </si>
+  <si>
+    <t>RC-3T15</t>
+  </si>
+  <si>
+    <t>RC-3T16</t>
+  </si>
+  <si>
+    <t>RC-3T17</t>
+  </si>
+  <si>
+    <t>RC-3T18</t>
   </si>
 </sst>
 </file>
@@ -385,7 +387,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -930,537 +932,633 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="47.796875" customWidth="1"/>
-    <col min="2" max="2" width="9.86328125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="4.796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="50.796875" style="13" customWidth="1"/>
-    <col min="6" max="6" width="9.86328125" customWidth="1"/>
-    <col min="7" max="7" width="6.1328125" customWidth="1"/>
+    <col min="1" max="1" width="47.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="50.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="15.75">
       <c r="A1" s="21" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="B1" s="21"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="15.75">
       <c r="A2" s="21" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="21"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="15.75">
       <c r="A3" s="17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7">
       <c r="A4" s="10" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B4" s="19"/>
     </row>
-    <row r="5" spans="1:7" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" ht="16.149999999999999" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75">
       <c r="A6" s="9"/>
       <c r="B6" s="14" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" ht="16.149999999999999" thickBot="1">
       <c r="A7" s="9" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="B7" s="15">
         <f>B8+F8</f>
-        <v>0</v>
+        <v>19.5</v>
       </c>
       <c r="C7" s="4">
         <f>C8+G8</f>
         <v>20</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="B8" s="7">
         <f>SUM(B9:B29)</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="C8" s="20">
         <f>SUM(C9:C29)</f>
         <v>10.5</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="F8" s="7">
         <f>SUM(F9:F29)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G8" s="20">
         <f>SUM(G9:G29)</f>
         <v>9.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0.5</v>
+      </c>
       <c r="C9" s="4">
         <v>0.5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="8"/>
+        <v>11</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.5</v>
+      </c>
       <c r="G9" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="8"/>
+        <v>12</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0.5</v>
+      </c>
       <c r="C10" s="4">
         <v>0.5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="8"/>
+        <v>13</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.5</v>
+      </c>
       <c r="G10" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="8"/>
+        <v>14</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.5</v>
+      </c>
       <c r="C11" s="4">
         <v>0.5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.5</v>
+      </c>
       <c r="G11" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0.25</v>
+      </c>
       <c r="C12" s="4">
         <v>0.25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="8"/>
+        <v>17</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.5</v>
+      </c>
       <c r="G12" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0.25</v>
+      </c>
       <c r="C13" s="4">
         <v>0.25</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.5</v>
+      </c>
       <c r="G13" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7">
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7">
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1.5</v>
+      </c>
       <c r="C17" s="4">
         <v>1.5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F17" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1</v>
+      </c>
       <c r="G17" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7">
       <c r="E18" s="1"/>
       <c r="F18" s="7"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:7" ht="15.75">
       <c r="A19" s="9" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B19" s="7"/>
       <c r="E19" s="9" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1.5</v>
+      </c>
       <c r="C21" s="4">
         <v>1.5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="F21" s="8">
+        <v>1</v>
+      </c>
       <c r="G21" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0.5</v>
+      </c>
       <c r="C22" s="18">
         <v>0.5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="8"/>
+        <v>31</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0.5</v>
+      </c>
       <c r="G22" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="8"/>
+        <v>32</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
       <c r="C23" s="4">
         <v>1</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="8"/>
+        <v>33</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0.75</v>
+      </c>
       <c r="G23" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="8"/>
+        <v>34</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1</v>
+      </c>
       <c r="C24" s="4">
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F24" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="F24" s="8">
+        <v>1</v>
+      </c>
       <c r="G24" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="B25" s="8">
+        <v>1</v>
+      </c>
       <c r="C25" s="4">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F25" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="F25" s="8">
+        <v>1</v>
+      </c>
       <c r="G25" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="8"/>
+        <v>38</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.5</v>
+      </c>
       <c r="C26" s="4">
         <v>0.5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" s="8"/>
+        <v>39</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0.5</v>
+      </c>
       <c r="G26" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="8"/>
+        <v>42</v>
+      </c>
+      <c r="B28" s="8">
+        <v>1.5</v>
+      </c>
       <c r="C28" s="4">
         <v>1.5</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" s="8"/>
+        <v>43</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.75</v>
+      </c>
       <c r="G28" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="43.9" customHeight="1">
       <c r="A31" s="22"/>
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
       <c r="D31" s="23"/>
       <c r="E31" s="24"/>
     </row>
-    <row r="32" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:7" ht="14.65" thickBot="1">
       <c r="A32" s="5"/>
       <c r="B32" s="12"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7">
       <c r="A33" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="4"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A34" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="8"/>
-      <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A35" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="8"/>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A36" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="G36" s="4"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="8"/>
-      <c r="G37" s="4"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A38" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="8"/>
-      <c r="G38" s="4"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="8"/>
-      <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A40" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="8"/>
-      <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A41" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="8"/>
-      <c r="G41" s="4"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A42" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="8"/>
-      <c r="G42" s="4"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" s="8"/>
-      <c r="G43" s="4"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A44" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="8"/>
-      <c r="G44" s="4"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A45" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="8"/>
-      <c r="G45" s="4"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" s="8"/>
+      <c r="B46" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G46" s="4"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7">
       <c r="A47" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" s="8"/>
+        <v>60</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G47" s="4"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7">
       <c r="A48" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48" s="8"/>
+        <v>61</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G48" s="4"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7">
       <c r="A49" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B49" s="8"/>
+        <v>62</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G49" s="4"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7">
       <c r="A50" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B50" s="8"/>
+        <v>63</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G50" s="4"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7">
       <c r="A51" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G51" s="4"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7">
       <c r="A52" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" s="8"/>
+        <v>65</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G52" s="4"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7">
       <c r="A53" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B53" s="8"/>
+        <v>66</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G53" s="4"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7">
       <c r="A54" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B54" s="8"/>
+        <v>67</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G54" s="4"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7">
       <c r="A55" s="16"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7">
       <c r="A56" s="16"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7">
       <c r="A57" s="16"/>
     </row>
   </sheetData>
@@ -1525,32 +1623,32 @@
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="9.796875" customWidth="1"/>
-    <col min="10" max="10" width="9.86328125" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:10">
       <c r="B2" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10">
       <c r="B3" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1562,12 +1660,12 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
       <c r="B4" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="D4">
         <v>0.25</v>
@@ -1579,12 +1677,12 @@
         <v>0.25</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
       <c r="B5" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="D5">
         <v>0.5</v>
@@ -1596,12 +1694,12 @@
         <v>0.5</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
       <c r="B6" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="F6">
         <v>0.75</v>
@@ -1610,12 +1708,12 @@
         <v>0.75</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1624,56 +1722,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:10">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="H8">
         <v>1.25</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="H9">
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:10">
       <c r="B10" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="H10">
         <v>1.75</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:10">
       <c r="B11" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:10">
       <c r="B12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
       <c r="B13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
       <c r="B14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
       <c r="B15" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1698,9 +1796,5 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58BB555B-AEAA-4A2D-82AD-47D916FBB73A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/DataMashup"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58BB555B-AEAA-4A2D-82AD-47D916FBB73A}"/>
 </file>
</xml_diff>